<commit_message>
Adicionando na planilha da tabela de produtos alguns itens para cadastrar no banco, adicionando tambem as imagens de cada produto na pasta public
</commit_message>
<xml_diff>
--- a/documentacao/Estrutura do Banco de Dados - Produtos.xlsx
+++ b/documentacao/Estrutura do Banco de Dados - Produtos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
   <si>
     <t>Produtos - Banco de Dados / P.I. EchoPet</t>
   </si>
@@ -134,12 +134,120 @@
   <si>
     <t>*Obs.: Adicionar a coluna pic_products_id para puxar a imagem do produto</t>
   </si>
+  <si>
+    <t>80.00</t>
+  </si>
+  <si>
+    <t>Ração vegetal para Cãaes Adultos Pedrigree</t>
+  </si>
+  <si>
+    <t>racaoPedrigree.jpg</t>
+  </si>
+  <si>
+    <t>Indicada para cães filhotes;</t>
+  </si>
+  <si>
+    <t>Nutrientes para um desenvolvimento saudavel;</t>
+  </si>
+  <si>
+    <t>Disponivel em embalagens de 5 kg;</t>
+  </si>
+  <si>
+    <t>Para cães de pequeno porte;</t>
+  </si>
+  <si>
+    <t>Vegetais naturais.</t>
+  </si>
+  <si>
+    <t>Barreiras antivazamento.</t>
+  </si>
+  <si>
+    <t>Super fino e leve;</t>
+  </si>
+  <si>
+    <t>30.00</t>
+  </si>
+  <si>
+    <t>45.00</t>
+  </si>
+  <si>
+    <t>50.00</t>
+  </si>
+  <si>
+    <t>Tamanho: 60 x 60 cm, contém 7 unidades no pac;</t>
+  </si>
+  <si>
+    <t>Biodegradável, ecologicamente correta;</t>
+  </si>
+  <si>
+    <t> Super econômica, dura até um mês;</t>
+  </si>
+  <si>
+    <t>Perfume agradável de lavanda;</t>
+  </si>
+  <si>
+    <t>Com partículas que inibem a proliferação de bactérias.</t>
+  </si>
+  <si>
+    <t>Areia_Sanitária_Gatos.jpg</t>
+  </si>
+  <si>
+    <t>Tapete_Higiênico_Cachorro.jpg</t>
+  </si>
+  <si>
+    <t>Tapetes Higienico PetLike para Cães 60 x 60 cm - 7 uni</t>
+  </si>
+  <si>
+    <t>Aréia Sanitária de Sílica Lavanda PetLike para Gatos</t>
+  </si>
+  <si>
+    <t>Ração Nutricon Nutriflakes para Peixes</t>
+  </si>
+  <si>
+    <t>65.00</t>
+  </si>
+  <si>
+    <t> Indicado para peixes em fase de crescimento ou manutenção;</t>
+  </si>
+  <si>
+    <t>Alimento em flocos para peixes ornamentais de água doce;</t>
+  </si>
+  <si>
+    <t>Melhora a resistências dos peixes;</t>
+  </si>
+  <si>
+    <t>Alimento saúdavel para o peixe.</t>
+  </si>
+  <si>
+    <t>Ração_Nutricon_Nutriflakes_para_Peixes.jpg</t>
+  </si>
+  <si>
+    <t>Ração Nutricon GoldFish Crescimento para Peixes - 400 g</t>
+  </si>
+  <si>
+    <t>Alimento extrusado flutuante;</t>
+  </si>
+  <si>
+    <t>Contribui para um bom desenvolvimento;</t>
+  </si>
+  <si>
+    <t>Realça as cores, devolvendo a beleza e o aspecto elegante;</t>
+  </si>
+  <si>
+    <t>Indicado para peixes de água fria kinguios e carpas em fase de crescimento.</t>
+  </si>
+  <si>
+    <t>Ração_Nutricon_GoldFish_Crescimento_para_Peixes.jpg</t>
+  </si>
+  <si>
+    <t>https://www.petlove.com.br/racao-nutricon-goldfish-crescimento-para-peixes-400-g/p</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +274,12 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -335,18 +449,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -364,12 +466,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -378,6 +474,34 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,79 +788,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M24"/>
+  <dimension ref="B2:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" style="1" customWidth="1"/>
     <col min="13" max="13" width="18.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="92.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
+      <c r="B4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="H5" s="18" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="H5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="20"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -754,7 +879,7 @@
       <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="11" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -774,7 +899,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="B7" s="5">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -798,7 +923,7 @@
       <c r="J7" s="2">
         <v>1</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="5">
         <v>1</v>
       </c>
       <c r="L7" s="3">
@@ -809,7 +934,7 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
+      <c r="B8" s="6">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -833,7 +958,7 @@
       <c r="J8" s="2">
         <v>1</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="5">
         <v>1</v>
       </c>
       <c r="L8" s="3">
@@ -844,7 +969,7 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="11">
+      <c r="B9" s="7">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -868,7 +993,7 @@
       <c r="J9" s="2">
         <v>1</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="5">
         <v>1</v>
       </c>
       <c r="L9" s="3">
@@ -879,7 +1004,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
+      <c r="B10" s="8">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -903,7 +1028,7 @@
       <c r="J10" s="2">
         <v>1</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="6">
         <v>2</v>
       </c>
       <c r="L10" s="3">
@@ -923,7 +1048,7 @@
       <c r="J11" s="2">
         <v>1</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="6">
         <v>2</v>
       </c>
       <c r="L11" s="3">
@@ -943,7 +1068,7 @@
       <c r="J12" s="2">
         <v>1</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="6">
         <v>2</v>
       </c>
       <c r="L12" s="3">
@@ -963,7 +1088,7 @@
       <c r="J13" s="2">
         <v>1</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="7">
         <v>3</v>
       </c>
       <c r="L13" s="3">
@@ -983,7 +1108,7 @@
       <c r="J14" s="2">
         <v>1</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="7">
         <v>3</v>
       </c>
       <c r="L14" s="3">
@@ -1003,7 +1128,7 @@
       <c r="J15" s="2">
         <v>1</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="7">
         <v>3</v>
       </c>
       <c r="L15" s="3">
@@ -1023,7 +1148,7 @@
       <c r="J16" s="2">
         <v>1</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="8">
         <v>4</v>
       </c>
       <c r="L16" s="3">
@@ -1033,7 +1158,7 @@
         <v>42494.729386574072</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H17" s="2">
         <v>11</v>
       </c>
@@ -1043,7 +1168,7 @@
       <c r="J17" s="2">
         <v>1</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="8">
         <v>4</v>
       </c>
       <c r="L17" s="3">
@@ -1053,7 +1178,7 @@
         <v>42494.729386574072</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H18" s="2">
         <v>12</v>
       </c>
@@ -1063,7 +1188,7 @@
       <c r="J18" s="2">
         <v>1</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="8">
         <v>4</v>
       </c>
       <c r="L18" s="3">
@@ -1073,68 +1198,71 @@
         <v>42494.729386574072</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="5" t="s">
+    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="7"/>
-    </row>
-    <row r="22" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="5" t="s">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="18"/>
+    </row>
+    <row r="22" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="7"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="14" t="s">
+      <c r="K23" s="10" t="s">
         <v>27</v>
       </c>
       <c r="L23" s="4" t="s">
@@ -1144,12 +1272,607 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="156" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
+    <row r="24" spans="2:14" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="16" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="21" t="s">
         <v>30</v>
+      </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+    </row>
+    <row r="25" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="21">
+        <v>1</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="21">
+        <v>1</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="21">
+        <v>50</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" s="21">
+        <v>3</v>
+      </c>
+      <c r="L25" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M25" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="21">
+        <v>2</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="21">
+        <v>1</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="21">
+        <v>60</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="22">
+        <v>1</v>
+      </c>
+      <c r="L26" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M26" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27" s="21">
+        <v>3</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="21">
+        <v>1</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="21">
+        <v>50</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="K27" s="21">
+        <v>4</v>
+      </c>
+      <c r="L27" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M27" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="B28" s="21">
+        <v>4</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="21">
+        <v>1</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="21">
+        <v>70</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" s="21">
+        <v>12</v>
+      </c>
+      <c r="L28" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M28" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="B29" s="21">
+        <v>5</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="21">
+        <v>1</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="21">
+        <v>70</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="K29" s="21">
+        <v>12</v>
+      </c>
+      <c r="L29" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M29" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="21">
+        <v>6</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M30" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="21">
+        <v>7</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M31" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="21">
+        <v>8</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M32" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="21">
+        <v>9</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M33" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="21">
+        <v>10</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M34" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="21">
+        <v>11</v>
+      </c>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M35" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="21">
+        <v>12</v>
+      </c>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M36" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="21">
+        <v>13</v>
+      </c>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M37" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="21">
+        <v>14</v>
+      </c>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M38" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="21">
+        <v>15</v>
+      </c>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M39" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="21">
+        <v>16</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M40" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="21">
+        <v>17</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M41" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="21">
+        <v>18</v>
+      </c>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M42" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="21">
+        <v>19</v>
+      </c>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M43" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="21">
+        <v>20</v>
+      </c>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M44" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="21">
+        <v>21</v>
+      </c>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M45" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="21">
+        <v>22</v>
+      </c>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M46" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="21">
+        <v>23</v>
+      </c>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M47" s="3">
+        <v>42494.729386574072</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="21">
+        <v>24</v>
+      </c>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="3">
+        <v>42494.729386574072</v>
+      </c>
+      <c r="M48" s="3">
+        <v>42494.729386574072</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizando a planilha de produtos para cadastrar via CRUD no banco / imagens salvas em public
</commit_message>
<xml_diff>
--- a/documentacao/Estrutura do Banco de Dados - Produtos.xlsx
+++ b/documentacao/Estrutura do Banco de Dados - Produtos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="187">
   <si>
     <t>Produtos - Banco de Dados / P.I. EchoPet</t>
   </si>
@@ -242,12 +242,369 @@
   <si>
     <t>https://www.petlove.com.br/racao-nutricon-goldfish-crescimento-para-peixes-400-g/p</t>
   </si>
+  <si>
+    <t>Ração Seca Nutrilus Pro Frango &amp; Carne para Cães Adultos</t>
+  </si>
+  <si>
+    <t>Proteínas de alta qualidade;</t>
+  </si>
+  <si>
+    <t>Redução do odor e firmeza das fezes;</t>
+  </si>
+  <si>
+    <t>Sem corantes e aromatizantes artificiais;</t>
+  </si>
+  <si>
+    <t>Enriquecido com vitaminas e minerais essenciais para maior saúde e vitalidade.</t>
+  </si>
+  <si>
+    <t>Ração_Seca_Nutrilus_Pro_Frango___Carne_para_Cães_Adultos</t>
+  </si>
+  <si>
+    <t>Tapete Higiênico Me.Au Pet para Cães</t>
+  </si>
+  <si>
+    <t> Tecnologia Slim: Super fino;</t>
+  </si>
+  <si>
+    <t>Atrativo Canino;</t>
+  </si>
+  <si>
+    <t>Sistema antirrasgo;</t>
+  </si>
+  <si>
+    <t>Tapete_Higiênico_Me.Au_Pet_para_Cães.jpg</t>
+  </si>
+  <si>
+    <t>Brinquedo American Pets Cat Toy Ratinho Arco-Íris</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>Diminui a ociosidade;</t>
+  </si>
+  <si>
+    <t>Combate o stress;</t>
+  </si>
+  <si>
+    <t>Estimula a atividade física.</t>
+  </si>
+  <si>
+    <t>Neutralizador de odores.</t>
+  </si>
+  <si>
+    <t>Atrativo para Gatos.</t>
+  </si>
+  <si>
+    <t>brinquedo_para_gato_reto.jpg</t>
+  </si>
+  <si>
+    <t>Alimento Zootekna Girassol Graúdo - 400 g</t>
+  </si>
+  <si>
+    <t>Rico em Proteínas, Óleos e Minerais;</t>
+  </si>
+  <si>
+    <t>Uso proibido na alimentação de ruminantes.</t>
+  </si>
+  <si>
+    <t>Para qualquer tipo de Pssáro;</t>
+  </si>
+  <si>
+    <t>Rende diversas porções.</t>
+  </si>
+  <si>
+    <t>comida_passaro_girassol.jpg</t>
+  </si>
+  <si>
+    <t>Ração Nutrópica Seleção Natural Calopsita</t>
+  </si>
+  <si>
+    <t>20.00</t>
+  </si>
+  <si>
+    <t>Alimento completo e balanceado;</t>
+  </si>
+  <si>
+    <t>Sabor insuperável com variedade de partículas extrusadas repletas de vitaminas e minerais;</t>
+  </si>
+  <si>
+    <t>Ração com probióticos que fortalecem seu pássaro;</t>
+  </si>
+  <si>
+    <t>Exclusiva combinação de 16 tipos de grãos integrais para sua ave consumir imediatamente.</t>
+  </si>
+  <si>
+    <t>Ração_Nutrópica_Seleção_Natural_Calopsita.jpg</t>
+  </si>
+  <si>
+    <t>Granulado Higiênico de Madeira Eco Farm</t>
+  </si>
+  <si>
+    <t>60.00</t>
+  </si>
+  <si>
+    <t>100% natural, biodegradável;</t>
+  </si>
+  <si>
+    <t>Não forma torrão, vira pó;</t>
+  </si>
+  <si>
+    <t>Mantém a gaiola seca e sem cheiro;</t>
+  </si>
+  <si>
+    <t>Pode ser descartado no vaso sanitário.</t>
+  </si>
+  <si>
+    <t>Granulado_Higiênico_de_Madeira_Eco_Farm.jpg</t>
+  </si>
+  <si>
+    <t>Areia Higiênica ProGato para Pássaros</t>
+  </si>
+  <si>
+    <t>Mais higiênico: Não faz lama e não forma torrão;</t>
+  </si>
+  <si>
+    <t>pH Neutro e atóxico: Não possui aditivos químicos;</t>
+  </si>
+  <si>
+    <t>Produto leve e alto rendimento: Maior rendimento com menos peso;</t>
+  </si>
+  <si>
+    <t>Fácil manutenção: Retirada apenas das fezes e dos grãos saturados.</t>
+  </si>
+  <si>
+    <t>Areia_Higiênica_ProGato_para_Pássaros_2022203_1.jpg</t>
+  </si>
+  <si>
+    <t>Comedouro Tudo Pet Automático Malha Fina para Pássaros</t>
+  </si>
+  <si>
+    <t>Fácil e prático de manusear;</t>
+  </si>
+  <si>
+    <t>Vazão adequada de alimentos;</t>
+  </si>
+  <si>
+    <t>Tampa hermética na base superior;</t>
+  </si>
+  <si>
+    <t>Bico longo e alto evitando derramamento.</t>
+  </si>
+  <si>
+    <t>Comedouro_Still_Pet_Automático_Malha_Fina_para_Pássaros_2415906.jpg</t>
+  </si>
+  <si>
+    <t>Removedor de Amônia Microbe Lift Nite Out II para Áquarios</t>
+  </si>
+  <si>
+    <t>Diminuição de amônia e nitrito;</t>
+  </si>
+  <si>
+    <t>Elimina a amônia através de um processo biológico natural chamado nitrificação.</t>
+  </si>
+  <si>
+    <t>Não armazenar em temperatura ambiente evitar a luz solar.</t>
+  </si>
+  <si>
+    <t>Preserva a saú do peixe;</t>
+  </si>
+  <si>
+    <t>Removedor_de_Amônia_Microbe_Lift_Nite_Out_II_para_Áquario.jpg</t>
+  </si>
+  <si>
+    <t>Suplemento Prodac Condicionar de Água Aquasana</t>
+  </si>
+  <si>
+    <t>Contém coloide natural que protege a mucosa da pele e as guelras;</t>
+  </si>
+  <si>
+    <t>Sua composição é rica em aloe vera;</t>
+  </si>
+  <si>
+    <t>Mantém o pH estável e equilibrado;</t>
+  </si>
+  <si>
+    <t>É um eficiente anti-stress.</t>
+  </si>
+  <si>
+    <t>Suplemento_Prodac_Condicionar_de_Água_Aquasana.jpg</t>
+  </si>
+  <si>
+    <t>Suplemento à Base de Fósforo Microbe Lift Phosphorus para Áquarios</t>
+  </si>
+  <si>
+    <t>Incentiva o crescimento das plantas exuberantes;</t>
+  </si>
+  <si>
+    <t>Fácil de usar suplemento líquido;</t>
+  </si>
+  <si>
+    <t>Sem nitrato;</t>
+  </si>
+  <si>
+    <t>Atrativo para os peixes.</t>
+  </si>
+  <si>
+    <t>Suplemento_à_Base_de_Fósforo_para_Áquarios.jpg</t>
+  </si>
+  <si>
+    <t>Ração Úmida Whiskas Sachê Frango ao Molho para Gatos Adultos</t>
+  </si>
+  <si>
+    <t>Suculentos pedacinhos cozidos a vapor;</t>
+  </si>
+  <si>
+    <t>Ajuda a manter a saúde do trato urinário;</t>
+  </si>
+  <si>
+    <t>Porção ideal de proteína, vitaminas e sais minerais;</t>
+  </si>
+  <si>
+    <t>Ração_Úmida_Whiskas_Sachê_Frango_ao_Molho_para_Gatos_Adultos.jpg</t>
+  </si>
+  <si>
+    <t>Ração Nestlé Purina Friskies Sachê Salmão ao Molho para Gatos</t>
+  </si>
+  <si>
+    <t>5.00</t>
+  </si>
+  <si>
+    <t>Alimento úmido completo e balanceado;</t>
+  </si>
+  <si>
+    <t>Sem conservantes, sem corantes artificiais e sem aromatizantes artificiais.</t>
+  </si>
+  <si>
+    <t>Destinado a gatos adultos;</t>
+  </si>
+  <si>
+    <t> Pronto para consumo;</t>
+  </si>
+  <si>
+    <t> Pedaços macios</t>
+  </si>
+  <si>
+    <t>Ração_Nestlé_Purina_Friskies_Sachê_Salmão_ao_Molho_para_Gatos.jpg</t>
+  </si>
+  <si>
+    <t>Brinquedo American Pets Bolinha Inteligente</t>
+  </si>
+  <si>
+    <t> Resistente;</t>
+  </si>
+  <si>
+    <t>Emite som ao ser chacoalhado;</t>
+  </si>
+  <si>
+    <t>De alta qualidade e durabilidade;</t>
+  </si>
+  <si>
+    <t>Furo para colocação de petisco, deixando a brincadeira mais divertida.</t>
+  </si>
+  <si>
+    <t>Bolinha_cachorro.jpg</t>
+  </si>
+  <si>
+    <t>Brinquedo Furacão Pet Dental Bone Algodão com Nó</t>
+  </si>
+  <si>
+    <t>Auxlia no combate ao tártaro;</t>
+  </si>
+  <si>
+    <t>Resistente;</t>
+  </si>
+  <si>
+    <t>Atrativo para o cão;</t>
+  </si>
+  <si>
+    <t>Mordida regular.</t>
+  </si>
+  <si>
+    <t>osso_no_cao.jpg</t>
+  </si>
+  <si>
+    <t>Brinquedo Interativo KONG Tunel Play Spaces Ca41 para Gatos - Vermelho</t>
+  </si>
+  <si>
+    <t>120.00</t>
+  </si>
+  <si>
+    <t>Dobrável para fácil armazenamento;</t>
+  </si>
+  <si>
+    <t>Estimula a curiosidade natural do seu gato;</t>
+  </si>
+  <si>
+    <t>É o brinquedo numero 1, indicado por veterinários do mundo todo, por seu apelo a incentivar o peludo a se exercitar com muita segurança com a durabilidade avançada de Kong;</t>
+  </si>
+  <si>
+    <t>Dobrável para fácil armazenamento.</t>
+  </si>
+  <si>
+    <t>brinquedo_interativo_gato.jpg</t>
+  </si>
+  <si>
+    <t>Lenços Umedecidos Pet Clean para Gatos</t>
+  </si>
+  <si>
+    <t>Com Aloe Vera;</t>
+  </si>
+  <si>
+    <t>Sem álcool;</t>
+  </si>
+  <si>
+    <t>Para limpeza a seco de gatos;</t>
+  </si>
+  <si>
+    <t>Auxilia na diminuição do efeito bola de pelo.</t>
+  </si>
+  <si>
+    <t>Lenços_Umedecidos_Pet_Clean_para_Gatos.jpg</t>
+  </si>
+  <si>
+    <t>Ração Nutral Carpa Crescimento e Cor - 300 g</t>
+  </si>
+  <si>
+    <t>Fórmula Balanceamento;</t>
+  </si>
+  <si>
+    <t>Crescimento Ideal;</t>
+  </si>
+  <si>
+    <t> Enriquecida com vitaminas e minerais.</t>
+  </si>
+  <si>
+    <t>Rende diversas porções, 300 g;</t>
+  </si>
+  <si>
+    <t>COR-CRESCIMENTO-300g-peixe.jpg</t>
+  </si>
+  <si>
+    <t>Mistura Balanceada Zootekna de Sementes Papagaio - 400 g</t>
+  </si>
+  <si>
+    <t>Livre de toxinas;</t>
+  </si>
+  <si>
+    <t>Aroma de frutas;</t>
+  </si>
+  <si>
+    <t>Indicada para Papagaios;</t>
+  </si>
+  <si>
+    <t>Porção de 400.</t>
+  </si>
+  <si>
+    <t>Mistura_Balanceada_Zootekna_de_Sementes_Papagaio_-_400_g.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +640,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4C4C4C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -437,7 +806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -466,6 +835,19 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,20 +869,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -790,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,54 +1204,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
     </row>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="18"/>
+      <c r="B4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="23"/>
     </row>
     <row r="5" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-      <c r="H5" s="12" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="H5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="14"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -1200,36 +1590,36 @@
     </row>
     <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="18"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="23"/>
     </row>
     <row r="22" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="18"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="23"/>
       <c r="N22" s="1" t="s">
         <v>67</v>
       </c>
@@ -1273,52 +1663,52 @@
       </c>
     </row>
     <row r="24" spans="2:14" ht="156" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="21" t="s">
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
     </row>
     <row r="25" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B25" s="21">
-        <v>1</v>
-      </c>
-      <c r="C25" s="21" t="s">
+      <c r="B25" s="14">
+        <v>1</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="21">
-        <v>1</v>
-      </c>
-      <c r="E25" s="21" t="s">
+      <c r="D25" s="14">
+        <v>1</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="14">
         <v>50</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="H25" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="I25" s="21" t="s">
+      <c r="I25" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="21" t="s">
+      <c r="J25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K25" s="21">
+      <c r="K25" s="27">
         <v>3</v>
       </c>
       <c r="L25" s="3">
@@ -1332,34 +1722,34 @@
       </c>
     </row>
     <row r="26" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B26" s="21">
+      <c r="B26" s="14">
         <v>2</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="21">
-        <v>1</v>
-      </c>
-      <c r="E26" s="21" t="s">
+      <c r="D26" s="14">
+        <v>1</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="14">
         <v>60</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="J26" s="21" t="s">
+      <c r="J26" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="28">
         <v>1</v>
       </c>
       <c r="L26" s="3">
@@ -1373,34 +1763,34 @@
       </c>
     </row>
     <row r="27" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="21">
+      <c r="B27" s="14">
         <v>3</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="21">
-        <v>1</v>
-      </c>
-      <c r="E27" s="21" t="s">
+      <c r="D27" s="14">
+        <v>1</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="14">
         <v>50</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="G27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H27" s="23" t="s">
+      <c r="H27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="I27" s="24" t="s">
+      <c r="I27" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="24" t="s">
+      <c r="J27" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="K27" s="21">
+      <c r="K27" s="29">
         <v>4</v>
       </c>
       <c r="L27" s="3">
@@ -1414,34 +1804,34 @@
       </c>
     </row>
     <row r="28" spans="2:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="B28" s="21">
+      <c r="B28" s="14">
         <v>4</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="21">
-        <v>1</v>
-      </c>
-      <c r="E28" s="21" t="s">
+      <c r="D28" s="14">
+        <v>1</v>
+      </c>
+      <c r="E28" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="14">
         <v>70</v>
       </c>
-      <c r="G28" s="24" t="s">
+      <c r="G28" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H28" s="24" t="s">
+      <c r="H28" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="I28" s="24" t="s">
+      <c r="I28" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="J28" s="21" t="s">
+      <c r="J28" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="K28" s="21">
+      <c r="K28" s="31">
         <v>12</v>
       </c>
       <c r="L28" s="3">
@@ -1455,34 +1845,34 @@
       </c>
     </row>
     <row r="29" spans="2:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="B29" s="21">
+      <c r="B29" s="14">
         <v>5</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="21">
-        <v>1</v>
-      </c>
-      <c r="E29" s="21" t="s">
+      <c r="D29" s="14">
+        <v>1</v>
+      </c>
+      <c r="E29" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="14">
         <v>70</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="H29" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I29" s="24" t="s">
+      <c r="I29" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="J29" s="24" t="s">
+      <c r="J29" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="K29" s="21">
+      <c r="K29" s="31">
         <v>12</v>
       </c>
       <c r="L29" s="3">
@@ -1495,384 +1885,783 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="21">
+    <row r="30" spans="2:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="B30" s="14">
         <v>6</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
+      <c r="C30" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="14">
+        <v>1</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="14">
+        <v>50</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" s="27">
+        <v>3</v>
+      </c>
       <c r="L30" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M30" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="21">
+      <c r="N30" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B31" s="14">
         <v>7</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
+      <c r="C31" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="14">
+        <v>1</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="14">
+        <v>55</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" s="27">
+        <v>1</v>
+      </c>
       <c r="L31" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M31" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="21">
+      <c r="N31" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B32" s="14">
         <v>8</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
+      <c r="C32" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="14">
+        <v>1</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="14">
+        <v>10</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="K32" s="29">
+        <v>5</v>
+      </c>
       <c r="L32" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M32" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="21">
+      <c r="N32" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="B33" s="14">
         <v>9</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
+      <c r="C33" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="14">
+        <v>1</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" s="14">
+        <v>20</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K33" s="30">
+        <v>9</v>
+      </c>
       <c r="L33" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M33" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="21">
+      <c r="N33" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="B34" s="14">
         <v>10</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
+      <c r="C34" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="14">
+        <v>1</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="14">
+        <v>30</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="K34" s="30">
+        <v>9</v>
+      </c>
       <c r="L34" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M34" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="21">
+      <c r="N34" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B35" s="14">
         <v>11</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
+      <c r="C35" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="14">
+        <v>1</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="14">
+        <v>20</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="K35" s="30">
+        <v>7</v>
+      </c>
       <c r="L35" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M35" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="21">
+      <c r="N35" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="B36" s="14">
         <v>12</v>
       </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
+      <c r="C36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="14">
+        <v>1</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="14">
+        <v>10</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="K36" s="30">
+        <v>7</v>
+      </c>
       <c r="L36" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M36" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="21">
+      <c r="N36" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B37" s="14">
         <v>13</v>
       </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
+      <c r="C37" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="14">
+        <v>1</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="14">
+        <v>15</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="K37" s="30">
+        <v>8</v>
+      </c>
       <c r="L37" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M37" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="21">
+      <c r="N37" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="B38" s="14">
         <v>14</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
+      <c r="C38" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="14">
+        <v>1</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="14">
+        <v>10</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="K38" s="31">
+        <v>10</v>
+      </c>
       <c r="L38" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M38" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="21">
+      <c r="N38" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="B39" s="14">
         <v>15</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
+      <c r="C39" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="14">
+        <v>1</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="14">
+        <v>10</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="I39" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="K39" s="31">
+        <v>10</v>
+      </c>
       <c r="L39" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M39" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="21">
+      <c r="N39" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="B40" s="14">
         <v>16</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
+      <c r="C40" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="14">
+        <v>1</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="14">
+        <v>15</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="K40" s="31">
+        <v>11</v>
+      </c>
       <c r="L40" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M40" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="21">
+      <c r="N40" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="B41" s="14">
         <v>17</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
+      <c r="C41" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="14">
+        <v>1</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" s="14">
+        <v>50</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="K41" s="29">
+        <v>6</v>
+      </c>
       <c r="L41" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M41" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="21">
+      <c r="N41" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B42" s="14">
         <v>18</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
+      <c r="C42" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" s="14">
+        <v>1</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F42" s="14">
+        <v>40</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="J42" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="K42" s="29">
+        <v>6</v>
+      </c>
       <c r="L42" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M42" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="21">
+      <c r="N42" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="B43" s="14">
         <v>19</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
+      <c r="C43" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D43" s="14">
+        <v>1</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="14">
+        <v>20</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="J43" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="K43" s="27">
+        <v>2</v>
+      </c>
       <c r="L43" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M43" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="21">
+      <c r="N43" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B44" s="14">
         <v>20</v>
       </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
+      <c r="C44" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="14">
+        <v>1</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" s="14">
+        <v>25</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="J44" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="K44" s="27">
+        <v>2</v>
+      </c>
       <c r="L44" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M44" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="21">
+      <c r="N44" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" ht="210" x14ac:dyDescent="0.25">
+      <c r="B45" s="14">
         <v>21</v>
       </c>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
+      <c r="C45" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="14">
+        <v>1</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="14">
+        <v>10</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="I45" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="K45" s="29">
+        <v>5</v>
+      </c>
       <c r="L45" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M45" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="21">
+      <c r="N45" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B46" s="14">
         <v>22</v>
       </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="21"/>
+      <c r="C46" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" s="14">
+        <v>1</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F46" s="14">
+        <v>20</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="I46" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="J46" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="K46" s="29">
+        <v>4</v>
+      </c>
       <c r="L46" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M46" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="21">
+      <c r="N46" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B47" s="14">
         <v>23</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
+      <c r="C47" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D47" s="14">
+        <v>1</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="14">
+        <v>30</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="J47" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="K47" s="31">
+        <v>12</v>
+      </c>
       <c r="L47" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M47" s="3">
         <v>42494.729386574072</v>
       </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="21">
+      <c r="N47" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="B48" s="14">
         <v>24</v>
       </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="21"/>
+      <c r="C48" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D48" s="14">
+        <v>1</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" s="14">
+        <v>50</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="K48" s="30">
+        <v>9</v>
+      </c>
       <c r="L48" s="3">
         <v>42494.729386574072</v>
       </c>
       <c r="M48" s="3">
         <v>42494.729386574072</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cadastrando produtos via CRUD para rodar o forEach
</commit_message>
<xml_diff>
--- a/documentacao/Estrutura do Banco de Dados - Produtos.xlsx
+++ b/documentacao/Estrutura do Banco de Dados - Produtos.xlsx
@@ -848,27 +848,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -892,6 +871,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M2"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,54 +1204,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="23"/>
+      <c r="B4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="31"/>
     </row>
     <row r="5" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="H5" s="17" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
+      <c r="H5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="19"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="27"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -1590,36 +1590,36 @@
     </row>
     <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="23"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31"/>
     </row>
     <row r="22" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="23"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="31"/>
       <c r="N22" s="1" t="s">
         <v>67</v>
       </c>
@@ -1681,7 +1681,7 @@
       <c r="M24" s="12"/>
     </row>
     <row r="25" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B25" s="14">
+      <c r="B25" s="24">
         <v>1</v>
       </c>
       <c r="C25" s="14" t="s">
@@ -1708,7 +1708,7 @@
       <c r="J25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K25" s="27">
+      <c r="K25" s="20">
         <v>3</v>
       </c>
       <c r="L25" s="3">
@@ -1722,7 +1722,7 @@
       </c>
     </row>
     <row r="26" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B26" s="14">
+      <c r="B26" s="24">
         <v>2</v>
       </c>
       <c r="C26" s="14" t="s">
@@ -1749,7 +1749,7 @@
       <c r="J26" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="28">
+      <c r="K26" s="21">
         <v>1</v>
       </c>
       <c r="L26" s="3">
@@ -1763,7 +1763,7 @@
       </c>
     </row>
     <row r="27" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="14">
+      <c r="B27" s="24">
         <v>3</v>
       </c>
       <c r="C27" s="14" t="s">
@@ -1790,7 +1790,7 @@
       <c r="J27" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="K27" s="29">
+      <c r="K27" s="22">
         <v>4</v>
       </c>
       <c r="L27" s="3">
@@ -1804,7 +1804,7 @@
       </c>
     </row>
     <row r="28" spans="2:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="B28" s="14">
+      <c r="B28" s="24">
         <v>4</v>
       </c>
       <c r="C28" s="16" t="s">
@@ -1831,7 +1831,7 @@
       <c r="J28" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="K28" s="31">
+      <c r="K28" s="24">
         <v>12</v>
       </c>
       <c r="L28" s="3">
@@ -1845,7 +1845,7 @@
       </c>
     </row>
     <row r="29" spans="2:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="B29" s="14">
+      <c r="B29" s="24">
         <v>5</v>
       </c>
       <c r="C29" s="16" t="s">
@@ -1872,7 +1872,7 @@
       <c r="J29" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="K29" s="31">
+      <c r="K29" s="24">
         <v>12</v>
       </c>
       <c r="L29" s="3">
@@ -1886,7 +1886,7 @@
       </c>
     </row>
     <row r="30" spans="2:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="B30" s="14">
+      <c r="B30" s="24">
         <v>6</v>
       </c>
       <c r="C30" s="16" t="s">
@@ -1913,7 +1913,7 @@
       <c r="J30" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="K30" s="27">
+      <c r="K30" s="20">
         <v>3</v>
       </c>
       <c r="L30" s="3">
@@ -1927,7 +1927,7 @@
       </c>
     </row>
     <row r="31" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B31" s="14">
+      <c r="B31" s="24">
         <v>7</v>
       </c>
       <c r="C31" s="16" t="s">
@@ -1954,7 +1954,7 @@
       <c r="J31" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="K31" s="27">
+      <c r="K31" s="20">
         <v>1</v>
       </c>
       <c r="L31" s="3">
@@ -1968,7 +1968,7 @@
       </c>
     </row>
     <row r="32" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B32" s="14">
+      <c r="B32" s="24">
         <v>8</v>
       </c>
       <c r="C32" s="16" t="s">
@@ -1983,7 +1983,7 @@
       <c r="F32" s="14">
         <v>10</v>
       </c>
-      <c r="G32" s="24" t="s">
+      <c r="G32" s="17" t="s">
         <v>81</v>
       </c>
       <c r="H32" s="16" t="s">
@@ -1995,7 +1995,7 @@
       <c r="J32" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="K32" s="29">
+      <c r="K32" s="22">
         <v>5</v>
       </c>
       <c r="L32" s="3">
@@ -2009,7 +2009,7 @@
       </c>
     </row>
     <row r="33" spans="2:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="B33" s="14">
+      <c r="B33" s="24">
         <v>9</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -2036,7 +2036,7 @@
       <c r="J33" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K33" s="30">
+      <c r="K33" s="23">
         <v>9</v>
       </c>
       <c r="L33" s="3">
@@ -2050,7 +2050,7 @@
       </c>
     </row>
     <row r="34" spans="2:14" ht="120" x14ac:dyDescent="0.25">
-      <c r="B34" s="14">
+      <c r="B34" s="24">
         <v>10</v>
       </c>
       <c r="C34" s="16" t="s">
@@ -2077,7 +2077,7 @@
       <c r="J34" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="K34" s="30">
+      <c r="K34" s="23">
         <v>9</v>
       </c>
       <c r="L34" s="3">
@@ -2091,7 +2091,7 @@
       </c>
     </row>
     <row r="35" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B35" s="14">
+      <c r="B35" s="24">
         <v>11</v>
       </c>
       <c r="C35" s="16" t="s">
@@ -2118,7 +2118,7 @@
       <c r="J35" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="K35" s="30">
+      <c r="K35" s="23">
         <v>7</v>
       </c>
       <c r="L35" s="3">
@@ -2132,7 +2132,7 @@
       </c>
     </row>
     <row r="36" spans="2:14" ht="105" x14ac:dyDescent="0.25">
-      <c r="B36" s="14">
+      <c r="B36" s="24">
         <v>12</v>
       </c>
       <c r="C36" s="16" t="s">
@@ -2159,7 +2159,7 @@
       <c r="J36" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="K36" s="30">
+      <c r="K36" s="23">
         <v>7</v>
       </c>
       <c r="L36" s="3">
@@ -2173,7 +2173,7 @@
       </c>
     </row>
     <row r="37" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B37" s="14">
+      <c r="B37" s="24">
         <v>13</v>
       </c>
       <c r="C37" s="16" t="s">
@@ -2200,7 +2200,7 @@
       <c r="J37" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="K37" s="30">
+      <c r="K37" s="23">
         <v>8</v>
       </c>
       <c r="L37" s="3">
@@ -2214,7 +2214,7 @@
       </c>
     </row>
     <row r="38" spans="2:14" ht="120" x14ac:dyDescent="0.25">
-      <c r="B38" s="14">
+      <c r="B38" s="24">
         <v>14</v>
       </c>
       <c r="C38" s="16" t="s">
@@ -2241,7 +2241,7 @@
       <c r="J38" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="K38" s="31">
+      <c r="K38" s="24">
         <v>10</v>
       </c>
       <c r="L38" s="3">
@@ -2255,10 +2255,10 @@
       </c>
     </row>
     <row r="39" spans="2:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="B39" s="14">
+      <c r="B39" s="24">
         <v>15</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="19" t="s">
         <v>125</v>
       </c>
       <c r="D39" s="14">
@@ -2282,7 +2282,7 @@
       <c r="J39" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="K39" s="31">
+      <c r="K39" s="24">
         <v>10</v>
       </c>
       <c r="L39" s="3">
@@ -2296,7 +2296,7 @@
       </c>
     </row>
     <row r="40" spans="2:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="B40" s="14">
+      <c r="B40" s="24">
         <v>16</v>
       </c>
       <c r="C40" s="16" t="s">
@@ -2323,7 +2323,7 @@
       <c r="J40" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="K40" s="31">
+      <c r="K40" s="24">
         <v>11</v>
       </c>
       <c r="L40" s="3">
@@ -2364,7 +2364,7 @@
       <c r="J41" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="K41" s="29">
+      <c r="K41" s="22">
         <v>6</v>
       </c>
       <c r="L41" s="3">
@@ -2402,10 +2402,10 @@
       <c r="I42" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="J42" s="26" t="s">
+      <c r="J42" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="K42" s="29">
+      <c r="K42" s="22">
         <v>6</v>
       </c>
       <c r="L42" s="3">
@@ -2446,7 +2446,7 @@
       <c r="J43" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="K43" s="27">
+      <c r="K43" s="20">
         <v>2</v>
       </c>
       <c r="L43" s="3">
@@ -2487,7 +2487,7 @@
       <c r="J44" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="K44" s="27">
+      <c r="K44" s="20">
         <v>2</v>
       </c>
       <c r="L44" s="3">
@@ -2528,7 +2528,7 @@
       <c r="J45" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="K45" s="29">
+      <c r="K45" s="22">
         <v>5</v>
       </c>
       <c r="L45" s="3">
@@ -2569,7 +2569,7 @@
       <c r="J46" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="K46" s="29">
+      <c r="K46" s="22">
         <v>4</v>
       </c>
       <c r="L46" s="3">
@@ -2586,7 +2586,7 @@
       <c r="B47" s="14">
         <v>23</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="19" t="s">
         <v>175</v>
       </c>
       <c r="D47" s="14">
@@ -2607,10 +2607,10 @@
       <c r="I47" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="J47" s="25" t="s">
+      <c r="J47" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="K47" s="31">
+      <c r="K47" s="24">
         <v>12</v>
       </c>
       <c r="L47" s="3">
@@ -2651,7 +2651,7 @@
       <c r="J48" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="K48" s="30">
+      <c r="K48" s="23">
         <v>9</v>
       </c>
       <c r="L48" s="3">

</xml_diff>